<commit_message>
adding bar chart, working on tooltips
</commit_message>
<xml_diff>
--- a/parent_deaths_condensed.xlsx
+++ b/parent_deaths_condensed.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="76">
   <si>
     <t>title</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>gender</t>
+  </si>
+  <si>
+    <t>Bolt</t>
   </si>
 </sst>
 </file>
@@ -589,11 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="88" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A22" zoomScale="88" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -617,7 +619,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -631,7 +633,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -645,7 +647,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -659,7 +661,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -673,7 +675,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -687,7 +689,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -701,7 +703,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -729,7 +731,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -743,7 +745,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -757,7 +759,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -771,7 +773,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -785,7 +787,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -799,7 +801,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -813,7 +815,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -827,7 +829,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -841,7 +843,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -855,7 +857,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -883,7 +885,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -897,7 +899,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -911,7 +913,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -939,7 +941,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -953,7 +955,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -967,7 +969,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -981,7 +983,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -995,7 +997,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -1009,7 +1011,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -1023,7 +1025,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>50</v>
       </c>
@@ -1037,7 +1039,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1051,7 +1053,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>53</v>
       </c>
@@ -1065,7 +1067,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -1079,7 +1081,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -1093,7 +1095,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>57</v>
       </c>
@@ -1107,7 +1109,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>58</v>
       </c>
@@ -1121,7 +1123,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>55</v>
       </c>
@@ -1135,7 +1137,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>57</v>
       </c>
@@ -1149,7 +1151,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>71</v>
       </c>
@@ -1163,7 +1165,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>28</v>
       </c>
@@ -1177,35 +1179,22 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="49" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="50" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="51" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="52" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="53" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="54" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="55" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="56" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="57" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>75</v>
+      </c>
+      <c r="B42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D57">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="both"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="3">
-      <filters>
-        <filter val="f"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:D57"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>